<commit_message>
more UI changes. Implemented date and by feild auto populization
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>to</t>
   </si>
@@ -74,6 +74,42 @@
   </si>
   <si>
     <t>dfAakSNatUDiGFZM</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>JS01</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Space Weed</t>
+  </si>
+  <si>
+    <t>SW420</t>
+  </si>
+  <si>
+    <t>kLi3pJdPSNnEaSk0</t>
+  </si>
+  <si>
+    <t>TO4</t>
+  </si>
+  <si>
+    <t>MAIN</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>l8fWIfXMgODcFPYQ</t>
   </si>
   <si>
     <t>asdfas</t>
@@ -152,7 +188,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -275,68 +311,114 @@
         <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>